<commit_message>
Extent reports Cross Browser testing Parallel testing Groups
</commit_message>
<xml_diff>
--- a/com.sevenrmartsupermarket/src/main/resources/Excel_Files/CreateDeliveryBoy.xlsx
+++ b/com.sevenrmartsupermarket/src/main/resources/Excel_Files/CreateDeliveryBoy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -165,6 +165,52 @@
   </si>
   <si>
     <t>patrizio11</t>
+  </si>
+  <si>
+    <t>Leo Clark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aholmes@hotmail.com </t>
+  </si>
+  <si>
+    <t>Flat 17z Anthony Track West Amyville OX12 8PJ</t>
+  </si>
+  <si>
+    <t>leoclrk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+595ed5c1</t>
+  </si>
+  <si>
+    <t>Laura Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tara.edwards@gray.com </t>
+  </si>
+  <si>
+    <t>83 Hill Trafficway New Dominic LL18 3RP</t>
+  </si>
+  <si>
+    <t>laurath</t>
+  </si>
+  <si>
+    <t>6d804f4a</t>
+  </si>
+  <si>
+    <t>Olivia Baker</t>
+  </si>
+  <si>
+    <t>reece.thompson@gmail.com</t>
+  </si>
+  <si>
+    <t>387 Edwards Corner Helenafort EX20 1ER</t>
+  </si>
+  <si>
+    <t>oliviaer</t>
+  </si>
+  <si>
+    <t>fdf5d389</t>
   </si>
 </sst>
 </file>
@@ -818,19 +864,26 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1150,10 +1203,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -1290,7 +1343,7 @@
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="1">
@@ -1307,16 +1360,16 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="8">
         <v>8028651281</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>37</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1327,7 +1380,7 @@
       </c>
     </row>
     <row r="9" ht="29" spans="1:6">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1336,7 +1389,7 @@
       <c r="C9" s="1">
         <v>7867311623</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -1347,7 +1400,7 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1364,6 +1417,66 @@
       </c>
       <c r="F10" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="11" ht="29" spans="1:6">
+      <c r="A11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="11">
+        <v>5371572860</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="11">
+        <v>5785483362</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="11">
+        <v>2263885888</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1377,6 +1490,9 @@
     <hyperlink ref="B10" r:id="rId7" display="patrizioDeRose@jourrapide.com" tooltip="mailto:patrizioDeRose@jourrapide.com"/>
     <hyperlink ref="B9" r:id="rId8" display="markusMoller@dayrep.com"/>
     <hyperlink ref="B8" r:id="rId9" display="rvbufford@claims.bufford.com"/>
+    <hyperlink ref="B11" r:id="rId10" display="aholmes@hotmail.com "/>
+    <hyperlink ref="B12" r:id="rId11" display="tara.edwards@gray.com "/>
+    <hyperlink ref="B13" r:id="rId12" display="reece.thompson@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>